<commit_message>
added risks, ethcal and legal issues
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spectre\Documents\OpenClassrooms_AI\fashion-insta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC28334E-00E7-4810-BD3E-DC391418C2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FC9BC94-20A6-417A-9DD7-165DE9DAB46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9B746B4F-FB1E-444B-8156-FB1C45738087}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9B746B4F-FB1E-444B-8156-FB1C45738087}"/>
   </bookViews>
   <sheets>
-    <sheet name="backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Kanban board" sheetId="2" r:id="rId2"/>
+    <sheet name="backlog" sheetId="4" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,8 +36,28 @@
 </workbook>
 </file>
 
+<file path=xl/python.xml><?xml version="1.0" encoding="utf-8"?>
+<python xmlns="http://schemas.microsoft.com/office/spreadsheetml/2023/python">
+  <environmentDefinition id="{882DD1B0-6546-4DFA-8A08-902A380B44EA}">
+    <initialization>
+      <code xml:space="preserve">import numpy as np
+import pandas as pd
+import matplotlib.pyplot as plt
+import seaborn as sns
+import statsmodels as sm
+import excel
+import warnings
+warnings.simplefilter('ignore')
+excel.set_xl_scalar_conversion(excel.convert_to_scalar)
+excel.set_xl_array_conversion(excel.convert_to_dataframe)
+</code>
+    </initialization>
+  </environmentDefinition>
+</python>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t>1. User Authentication &amp; Profile Management</t>
   </si>
@@ -241,12 +261,133 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <t>Title...</t>
+  </si>
+  <si>
+    <t>As a...</t>
+  </si>
+  <si>
+    <t>I want to...</t>
+  </si>
+  <si>
+    <t>in order to...</t>
+  </si>
+  <si>
+    <t>Weight...</t>
+  </si>
+  <si>
+    <t>Required data...</t>
+  </si>
+  <si>
+    <t>User Authentication &amp; Profile Management</t>
+  </si>
+  <si>
+    <t>Application user</t>
+  </si>
+  <si>
+    <t>access my personalized shopping experience.</t>
+  </si>
+  <si>
+    <t>securely register and log in using email, phone, or social accounts.</t>
+  </si>
+  <si>
+    <t>Users email
+User's phone number, or
+User's username.</t>
+  </si>
+  <si>
+    <t>Photo Upload &amp; Wardrobe Capture</t>
+  </si>
+  <si>
+    <t>upload photos of my clothing and outfits</t>
+  </si>
+  <si>
+    <t>have the app build a personal wardrobe catalog</t>
+  </si>
+  <si>
+    <t>Outfit Recommendation Engine</t>
+  </si>
+  <si>
+    <t>the app to suggest outfit combinations from my wardrobe for a given occasion and weather</t>
+  </si>
+  <si>
+    <t>choose what to buy quickly</t>
+  </si>
+  <si>
+    <t>Virtual Try-On / Outfit Preview</t>
+  </si>
+  <si>
+    <t>virtually preview outfits on my uploaded photo or avatar</t>
+  </si>
+  <si>
+    <t>see how combinations look before buying them.</t>
+  </si>
+  <si>
+    <t>Personalization &amp; Learning</t>
+  </si>
+  <si>
+    <t>User's photos</t>
+  </si>
+  <si>
+    <t>have the app learn my style preferences over time</t>
+  </si>
+  <si>
+    <t>User's photos,
+Catalog photos
+Model training &amp; testing data</t>
+  </si>
+  <si>
+    <t>Model training &amp; testing data</t>
+  </si>
+  <si>
+    <t>for recommendations to improve with my feedback</t>
+  </si>
+  <si>
+    <t>Shopping Cart &amp; Checkout</t>
+  </si>
+  <si>
+    <t>add products to my cart and complete purchases using multiple payment methods</t>
+  </si>
+  <si>
+    <t>shop conveniently</t>
+  </si>
+  <si>
+    <t>Catalog Photos,
+Shopping cart,
+User's payment information,
+User's shipping information</t>
+  </si>
+  <si>
+    <t>Order Tracking</t>
+  </si>
+  <si>
+    <t>track my order status in real-time</t>
+  </si>
+  <si>
+    <t>know when my purchase will arrive</t>
+  </si>
+  <si>
+    <t>tracking information</t>
+  </si>
+  <si>
+    <t>Push Notifications &amp; Promotions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> receive notifications about offers and order updates</t>
+  </si>
+  <si>
+    <t>stay informed and engaged</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,16 +422,40 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -298,11 +463,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -325,6 +505,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,6 +532,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -658,11 +854,240 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E13670-4240-4674-8EF5-150D8A1F9C5B}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="8">
+        <v>8</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="9">
+        <v>13</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="8">
+        <v>8</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="9">
+        <v>13</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="8">
+        <v>13</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="9">
+        <v>8</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="8">
+        <v>8</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="9">
+        <v>5</v>
+      </c>
+      <c r="G9" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBAE6761-8268-4C66-B799-6754DEC0483A}">
   <dimension ref="A1:A61"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,16 +1373,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA59F42D-34DB-48AA-B9A1-519759B806B1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>